<commit_message>
add list of figures and codes
</commit_message>
<xml_diff>
--- a/Bac2Feature_codes_for_experiments.xlsx
+++ b/Bac2Feature_codes_for_experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fuyo/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69909034-3D30-8046-8D09-E1BD3589B38F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73C48BC-4AFE-0E47-9846-74F2855BCA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="1140" windowWidth="27900" windowHeight="16860" xr2:uid="{DE342C58-8678-8346-9C54-FC1C5005347F}"/>
   </bookViews>
@@ -102,18 +102,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>https://github.com/fuyo780/Bac2Feature_experiment/scripts/02_data_preprocessing/02_data_preprocessing.ipynb</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>https://github.com/fuyo780/Bac2Feature_experiment/scripts/02_data_preprocessing/02_visualization.R.ipynb</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>https://github.com/fuyo780/Bac2Feature_experiment/scripts/03_cross_validation/03_cross_validation.ipynb</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Bac2Feature_experiment/scripts/04_runtime_benchmarking/04_runtime_benchmarking.ipynb</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -122,14 +110,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>https://github.com/fuyo780/Bac2Feature_experiment/scripts/04_runtime_benchmarking/04_runtime_benchmarking.ipynb</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>https://github.com/fuyo780/Bac2Feature_experiment/scripts/05_phylogenetic_signals/05_phylogenetic_signals.ipynb</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Figure 3b</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -142,18 +122,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>https://github.com/fuyo780/Bac2Feature_experiment/scripts/06_trait_autocorrelations/06_trait_autocorrelations.ipynb</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Bac2Feature_experiment/scripts/07_application_gutmicrobiome/07_application_gutmicrobiome.ipynb</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>https://github.com/fuyo780/Bac2Feature_experiment/scripts/07_application_gutmicrobiome/07_application_gutmicrobiome.ipynb</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Figure 4a</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -167,6 +139,34 @@
   </si>
   <si>
     <t>Figure 4d</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://github.com/fuyo780/Bac2Feature_experiment/blob/main/scripts/02_data_preprocessing/02_dataset_preprocessing.ipynb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://github.com/fuyo780/Bac2Feature_experiment/blob/main/scripts/02_data_preprocessing/02_visualization.R.ipynb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://github.com/fuyo780/Bac2Feature_experiment/blob/main/scripts/03_cross_validation/03_cross_validation.ipynb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://github.com/fuyo780/Bac2Feature_experiment/blob/main/scripts/04_runtime_benchmarking/04_runtime_benchmarking.ipynb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://github.com/fuyo780/Bac2Feature_experiment/blob/main/scripts/05_phylogenetic_signals/05_phylogenetic_signals.ipynb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://github.com/fuyo780/Bac2Feature_experiment/blob/main/scripts/06_trait_autocorrelations/06_trait_autocorrelations.ipynb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://github.com/fuyo780/Bac2Feature_experiment/blob/main/scripts/07_application_gutmicrobiome/07_application_gutmicrobiome.ipynb</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -615,14 +615,14 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="77" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="107.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="124.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -649,7 +649,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -660,7 +660,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -671,7 +671,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -682,7 +682,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -693,7 +693,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -704,7 +704,7 @@
         <v>15</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -712,10 +712,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -723,10 +723,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -734,96 +734,96 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" xr:uid="{1F5C44D3-A848-2E4A-B0DD-73D87D5F12C6}"/>
-    <hyperlink ref="C6" r:id="rId2" xr:uid="{12778F4E-5FE3-5043-88EA-B84B00F320C7}"/>
-    <hyperlink ref="C10" r:id="rId3" xr:uid="{F9D82319-B174-EE4E-A1AC-2183A85D6DC7}"/>
-    <hyperlink ref="C8" r:id="rId4" xr:uid="{CCF56BCC-8A5E-2E47-A8CE-3F08E92899F9}"/>
-    <hyperlink ref="C9" r:id="rId5" xr:uid="{BAE76D8A-4F66-6348-8661-21AAE8DEFF99}"/>
-    <hyperlink ref="C5" r:id="rId6" xr:uid="{B71090D4-5825-7342-98FB-54309B68E8E0}"/>
-    <hyperlink ref="C7" r:id="rId7" xr:uid="{137D8550-6264-EE4C-9648-6671BDA20EFF}"/>
-    <hyperlink ref="C11" r:id="rId8" xr:uid="{606E5A74-AABF-B34B-812A-94DB0F4E70AE}"/>
-    <hyperlink ref="C12" r:id="rId9" xr:uid="{EAA35332-D9DF-F44C-B211-3B7729E51B2E}"/>
-    <hyperlink ref="C13" r:id="rId10" xr:uid="{7E8556CF-2A37-AE4A-9ECA-BAC003A24577}"/>
-    <hyperlink ref="C14" r:id="rId11" xr:uid="{FDB9FCF5-7526-3946-81F4-F354FC05B63C}"/>
-    <hyperlink ref="C15" r:id="rId12" xr:uid="{32EFEEF7-0946-A448-A092-715ABAFBF18F}"/>
-    <hyperlink ref="C16" r:id="rId13" xr:uid="{D92D5D2F-FD1C-B447-85C2-2F8C49BB2946}"/>
-    <hyperlink ref="C17" r:id="rId14" xr:uid="{F7ED3C90-B778-A64E-A848-E98578C52870}"/>
-    <hyperlink ref="C18" r:id="rId15" xr:uid="{474C89B3-1843-4B42-A152-8FAE5E22A513}"/>
+    <hyperlink ref="C6" r:id="rId1" xr:uid="{12778F4E-5FE3-5043-88EA-B84B00F320C7}"/>
+    <hyperlink ref="C10" r:id="rId2" xr:uid="{F9D82319-B174-EE4E-A1AC-2183A85D6DC7}"/>
+    <hyperlink ref="C8" r:id="rId3" xr:uid="{CCF56BCC-8A5E-2E47-A8CE-3F08E92899F9}"/>
+    <hyperlink ref="C9" r:id="rId4" xr:uid="{BAE76D8A-4F66-6348-8661-21AAE8DEFF99}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{B71090D4-5825-7342-98FB-54309B68E8E0}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{137D8550-6264-EE4C-9648-6671BDA20EFF}"/>
+    <hyperlink ref="C11" r:id="rId7" xr:uid="{606E5A74-AABF-B34B-812A-94DB0F4E70AE}"/>
+    <hyperlink ref="C12" r:id="rId8" xr:uid="{EAA35332-D9DF-F44C-B211-3B7729E51B2E}"/>
+    <hyperlink ref="C13" r:id="rId9" xr:uid="{7E8556CF-2A37-AE4A-9ECA-BAC003A24577}"/>
+    <hyperlink ref="C14" r:id="rId10" xr:uid="{FDB9FCF5-7526-3946-81F4-F354FC05B63C}"/>
+    <hyperlink ref="C15" r:id="rId11" xr:uid="{32EFEEF7-0946-A448-A092-715ABAFBF18F}"/>
+    <hyperlink ref="C16" r:id="rId12" xr:uid="{D92D5D2F-FD1C-B447-85C2-2F8C49BB2946}"/>
+    <hyperlink ref="C17" r:id="rId13" xr:uid="{F7ED3C90-B778-A64E-A848-E98578C52870}"/>
+    <hyperlink ref="C18" r:id="rId14" xr:uid="{474C89B3-1843-4B42-A152-8FAE5E22A513}"/>
+    <hyperlink ref="C4" r:id="rId15" xr:uid="{238B733E-735B-CD45-883E-F741DA5D7807}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
modified list of codes
</commit_message>
<xml_diff>
--- a/Bac2Feature_codes_for_experiments.xlsx
+++ b/Bac2Feature_codes_for_experiments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fuyo/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73C48BC-4AFE-0E47-9846-74F2855BCA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2738943E-2C3C-C640-AE3A-3D8AE98E0C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="1140" windowWidth="27900" windowHeight="16860" xr2:uid="{DE342C58-8678-8346-9C54-FC1C5005347F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
   <si>
     <t>List of codes used in this study</t>
     <phoneticPr fontId="1"/>
@@ -167,6 +167,66 @@
   </si>
   <si>
     <t>https://github.com/fuyo780/Bac2Feature_experiment/blob/main/scripts/07_application_gutmicrobiome/07_application_gutmicrobiome.ipynb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Figure 5a</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Bac2Feature_experiment/scripts/08_application_lakesoilmicrobiome/08_application_lakesoilmicrobiome.ipynb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://github.com/fuyo780/Bac2Feature_experiment/blob/main/scripts/08_application_lakesoilmicrobiome/08_application_lakesoilmicrobiome.ipynb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Figure 5b</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Bac2Feature_experiment/scripts/09_cross_validation_suppl/092_homology/092_compare_homology_based_prediction.ipynb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://github.com/fuyo780/Bac2Feature_experiment/blob/main/scripts/09_cross_validation_suppl/092_homology/092_compare_homology_based_prediction.ipynb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Bac2Feature_experiment/scripts/09_cross_validation_suppl/091_taxonomy/091_compare_taxonomic_classifier.ipynb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://github.com/fuyo780/Bac2Feature_experiment/blob/main/scripts/09_cross_validation_suppl/091_taxonomy/091_compare_taxonomic_classifier.ipynb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Bac2Feature_experiment/scripts/09_cross_validation_suppl/093_phylogeny/093_compare_hsp_method.ipynb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://github.com/fuyo780/Bac2Feature_experiment/blob/main/scripts/09_cross_validation_suppl/093_phylogeny/093_compare_hsp_method.ipynb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Figure S7</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Bac2Feature_experiment/scripts/09_cross_validation_suppl/094_clade_out/094_clade_out_cross_validation.ipynb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://github.com/fuyo780/Bac2Feature_experiment/blob/main/scripts/09_cross_validation_suppl/094_clade_out/094_clade_out_cross_validation.ipynb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Figure S5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Figure S6</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -216,6 +276,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -612,17 +673,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA0D6F48-EECA-BE49-BEEE-71E3CD2FCA82}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="77" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="124.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="144.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -686,8 +747,8 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="5" t="s">
-        <v>7</v>
+      <c r="A8" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>15</v>
@@ -697,8 +758,8 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="5" t="s">
-        <v>8</v>
+      <c r="A9" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>15</v>
@@ -804,6 +865,72 @@
       </c>
       <c r="C18" s="4" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -824,6 +951,12 @@
     <hyperlink ref="C17" r:id="rId13" xr:uid="{F7ED3C90-B778-A64E-A848-E98578C52870}"/>
     <hyperlink ref="C18" r:id="rId14" xr:uid="{474C89B3-1843-4B42-A152-8FAE5E22A513}"/>
     <hyperlink ref="C4" r:id="rId15" xr:uid="{238B733E-735B-CD45-883E-F741DA5D7807}"/>
+    <hyperlink ref="C19" r:id="rId16" xr:uid="{7FE7BCD8-6010-1F4E-BF4B-2162D06E7B01}"/>
+    <hyperlink ref="C22" r:id="rId17" xr:uid="{53296750-A9F6-A946-B71A-4068FD4CF9F6}"/>
+    <hyperlink ref="C23" r:id="rId18" xr:uid="{4D1B3EDB-C0A2-BD43-BFD1-4565EA012F8D}"/>
+    <hyperlink ref="C24" r:id="rId19" xr:uid="{EE6BBCCF-1020-E44F-8A6E-F18327291C13}"/>
+    <hyperlink ref="C20" r:id="rId20" xr:uid="{389AB43E-7437-1642-8BE1-FDB04C42C27A}"/>
+    <hyperlink ref="C21" r:id="rId21" xr:uid="{56870AF6-56B6-7541-98A5-A69268A2BB51}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>